<commit_message>
[FIX] #2616 report register of guarantee
</commit_message>
<xml_diff>
--- a/pabi_account_report/xlsx_template/xlsx_report_registrar_of_guarantee.xlsx
+++ b/pabi_account_report/xlsx_template/xlsx_report_registrar_of_guarantee.xlsx
@@ -88,13 +88,13 @@
     <t xml:space="preserve">Voucher Text</t>
   </si>
   <si>
-    <t xml:space="preserve">เลขที่สัญญา</t>
+    <t xml:space="preserve">Contract Number</t>
   </si>
   <si>
-    <t xml:space="preserve">วันที่เริ่มต้นสัญญา</t>
+    <t xml:space="preserve">Contract Start Date</t>
   </si>
   <si>
-    <t xml:space="preserve">วันที่สิ้นสุดสัญญา</t>
+    <t xml:space="preserve">Contract End Date</t>
   </si>
   <si>
     <t xml:space="preserve">ประเภทเงินค้ำประกัน</t>
@@ -319,8 +319,8 @@
   </sheetPr>
   <dimension ref="A1:AMJ12"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="L14" activeCellId="0" sqref="L14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -340,9 +340,9 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="3" width="15.23"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="2" width="20.56"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="4" width="13.92"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="4" width="24.59"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="4" width="24.6"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="2" width="22.09"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="2" width="21.81"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="2" width="21.82"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="2" width="18.47"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="2" width="20.98"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1023" min="21" style="5" width="11.52"/>

</xml_diff>